<commit_message>
updated 10/11 with resource scores
</commit_message>
<xml_diff>
--- a/notebooks/libraries_updated.xlsx
+++ b/notebooks/libraries_updated.xlsx
@@ -668,7 +668,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Edgehill</t>
+          <t>Edgehill Library</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bellevue</t>
+          <t>Bellevue Library</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1104,7 +1104,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Bordeaux Library</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1330,7 +1330,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>East</t>
+          <t>East Library</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Edmondson Pike</t>
+          <t>Edmondson Pike Library</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1767,7 +1767,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Goodlettsville</t>
+          <t>Goodlettsville Library</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1973,7 +1973,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Green Hills</t>
+          <t>Green Hills Library</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2199,7 +2199,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hadley Park</t>
+          <t>Hadley Park Library</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2409,7 +2409,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hermitage </t>
+          <t>Hermitage  Library</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2635,7 +2635,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Inglewood</t>
+          <t>Inglewood Library</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2845,7 +2845,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Looby</t>
+          <t>Looby Library</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3055,7 +3055,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Madison</t>
+          <t>Madison Library</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3281,7 +3281,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>North</t>
+          <t>North Library</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3491,7 +3491,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Old Hickory</t>
+          <t>Old Hickory Library</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3701,7 +3701,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Pruitt</t>
+          <t>Pruitt Library</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3911,7 +3911,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Richland Park</t>
+          <t>Richland Park Library</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -4121,7 +4121,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Southeast </t>
+          <t>Southeast  Library</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -4347,7 +4347,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Thompson Lane</t>
+          <t>Thompson Lane Library</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4557,7 +4557,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Watkins Park</t>
+          <t>Watkins Park Library</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4760,7 +4760,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Donelson</t>
+          <t>Donelson Library</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -4970,7 +4970,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Main</t>
+          <t>Main Library</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">

</xml_diff>